<commit_message>
Escritura y borrado en la mayor parte de Excel
</commit_message>
<xml_diff>
--- a/JavaApplication19/src/excel/Equipo.xlsx
+++ b/JavaApplication19/src/excel/Equipo.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="147">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -430,6 +430,48 @@
   </si>
   <si>
     <t>23  julio</t>
+  </si>
+  <si>
+    <t>24  julio</t>
+  </si>
+  <si>
+    <t>Martillo Nuevesini</t>
+  </si>
+  <si>
+    <t>Martillo para golpear bici</t>
+  </si>
+  <si>
+    <t>$250</t>
+  </si>
+  <si>
+    <t>Desarmador de estrella</t>
+  </si>
+  <si>
+    <t>Desarmador tipo estrella</t>
+  </si>
+  <si>
+    <t>$500</t>
+  </si>
+  <si>
+    <t>Martillo Nuevo</t>
+  </si>
+  <si>
+    <t>Equisde</t>
+  </si>
+  <si>
+    <t>$150</t>
+  </si>
+  <si>
+    <t>Llave Allen</t>
+  </si>
+  <si>
+    <t>Llave para apretars</t>
+  </si>
+  <si>
+    <t>$8000</t>
+  </si>
+  <si>
+    <t>$58000</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1234,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
@@ -1869,43 +1911,70 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="15">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s" s="15">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s" s="15">
+        <v>135</v>
+      </c>
+      <c r="D53" t="s" s="15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="15">
+        <v>133</v>
+      </c>
+      <c r="B54" t="s" s="15">
+        <v>137</v>
+      </c>
+      <c r="C54" t="s" s="15">
+        <v>138</v>
+      </c>
+      <c r="D54" t="s" s="15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="15">
+        <v>133</v>
+      </c>
+      <c r="B55" t="s" s="15">
         <v>126</v>
       </c>
-      <c r="C53" t="s" s="15">
+      <c r="C55" t="s" s="15">
         <v>127</v>
       </c>
-      <c r="D53" t="s" s="15">
+      <c r="D55" t="s" s="15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="15">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s" s="15">
+        <v>126</v>
+      </c>
+      <c r="C56" t="s" s="15">
+        <v>127</v>
+      </c>
+      <c r="D56" t="s" s="15">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="17">
+    <row r="57" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="17">
         <f>SUM(D2:D43)</f>
         <v>10563.19</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="D58" s="1"/>
@@ -2085,22 +2154,22 @@
       <c r="B93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="D97" s="1"/>
@@ -2140,35 +2209,15 @@
       <c r="B104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="D106" s="1"/>
-    </row>
-    <row r="107" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="D107" s="1"/>
-    </row>
-    <row r="108" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="D110" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D44">

</xml_diff>